<commit_message>
Fix stacked revenue chart and add multi-market revenue projection section
Add BESS revenue projection as lead section with stacked bar chart showing
revenue breakdown by market source (aFRR, FCR, DA, mFRR, Imbalance).
Fix Plotly chart rendering bug where mixed numeric/string x-axis labels
caused bars to collapse by forcing xaxis type to 'category'.
Replace static HTML reports with dynamic Plotly version.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/BirdEnergySystemInstalled_Lithuania.xlsx
+++ b/BirdEnergySystemInstalled_Lithuania.xlsx
@@ -691,7 +691,6 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -1744,10 +1743,11 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Retrieved: 2026-02-12 11:47 | Source: ENTSO-E Transparency Platform API</t>
-        </is>
-      </c>
-    </row>
+          <t>Retrieved: 2026-02-12 13:39 | Source: ENTSO-E Transparency Platform API</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
@@ -1953,6 +1953,7 @@
         <v>4025</v>
       </c>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
@@ -2106,6 +2107,7 @@
         <v>98.06</v>
       </c>
     </row>
+    <row r="23"/>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
@@ -2245,6 +2247,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31"/>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
@@ -2424,6 +2427,7 @@
         <v>1.95</v>
       </c>
     </row>
+    <row r="41"/>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
@@ -2759,6 +2763,7 @@
         <v>13.673</v>
       </c>
     </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
@@ -5777,7 +5782,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
@@ -6001,7 +6005,6 @@
         </is>
       </c>
     </row>
-    <row r="24"/>
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
@@ -6198,7 +6201,6 @@
         </is>
       </c>
     </row>
-    <row r="33"/>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
@@ -6440,24 +6442,6 @@
         <v>410</v>
       </c>
     </row>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
         <is>
@@ -6711,7 +6695,6 @@
         </is>
       </c>
     </row>
-    <row r="68"/>
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
         <is>
@@ -9923,4 +9906,231 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100109F5098D56F424FA4AE2D5DB3775DD9" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bcef5a2efb510c0d754b8a5c10a84197">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd59a36f-f5b4-4661-855e-b7d863e80f5b" xmlns:ns3="403ded9a-4eda-43f8-ae6e-341565e75e50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="27ca7bd51a5e75cd568ba3313fccdefe" ns2:_="" ns3:_="">
+    <xsd:import namespace="bd59a36f-f5b4-4661-855e-b7d863e80f5b"/>
+    <xsd:import namespace="403ded9a-4eda-43f8-ae6e-341565e75e50"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bd59a36f-f5b4-4661-855e-b7d863e80f5b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Afbeeldingtags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="723c8fce-9c0a-44c2-a82d-702bc7936f43" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="403ded9a-4eda-43f8-ae6e-341565e75e50" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{917f1675-4eb3-4acc-b1e3-455ddbc2a688}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="403ded9a-4eda-43f8-ae6e-341565e75e50">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="403ded9a-4eda-43f8-ae6e-341565e75e50" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bd59a36f-f5b4-4661-855e-b7d863e80f5b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77A0CB7D-74E3-442E-B608-89FBA76F5903}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E80D4B42-D3B9-4DBF-A204-B02A24FEFEED}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1492EFD-9552-4E83-91F6-34D209584F42}"/>
 </file>
</xml_diff>